<commit_message>
add code to create and run deterministic runs -- OM not working now
</commit_message>
<xml_diff>
--- a/case list.xlsx
+++ b/case list.xlsx
@@ -142,18 +142,12 @@
     <t>D103</t>
   </si>
   <si>
-    <t>Age and length comps</t>
-  </si>
-  <si>
     <t>Length comps only</t>
   </si>
   <si>
     <t>length and conditional age-at-length</t>
   </si>
   <si>
-    <t xml:space="preserve">Age, length and CAL </t>
-  </si>
-  <si>
     <t>D0 but with CAL data</t>
   </si>
   <si>
@@ -164,6 +158,12 @@
   </si>
   <si>
     <t>Same as D100 but w/o age data</t>
+  </si>
+  <si>
+    <t>Age and length comps, deterministic</t>
+  </si>
+  <si>
+    <t>Length and calcomps, deterministic</t>
   </si>
 </sst>
 </file>
@@ -527,7 +527,7 @@
   <dimension ref="B1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -683,10 +683,10 @@
         <v>38</v>
       </c>
       <c r="C14" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G14" s="1"/>
     </row>
@@ -695,10 +695,10 @@
         <v>39</v>
       </c>
       <c r="C15" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="D15" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G15" s="1"/>
     </row>
@@ -707,10 +707,10 @@
         <v>40</v>
       </c>
       <c r="C16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D16" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G16" s="1"/>
     </row>
@@ -719,10 +719,10 @@
         <v>41</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D17" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
first pass at results for determinstic cases
</commit_message>
<xml_diff>
--- a/case list.xlsx
+++ b/case list.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="360" windowWidth="15980" windowHeight="6110"/>
+    <workbookView xWindow="684" yWindow="360" windowWidth="15984" windowHeight="6108"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="67">
   <si>
     <t>F0</t>
   </si>
@@ -124,12 +124,6 @@
     <t>Same as D3 but with CAL instead of Age for survey</t>
   </si>
   <si>
-    <t>to use in combination with calcomp6</t>
-  </si>
-  <si>
-    <t>to use in combination with calcomp7</t>
-  </si>
-  <si>
     <t>D100</t>
   </si>
   <si>
@@ -139,38 +133,95 @@
     <t>D102</t>
   </si>
   <si>
-    <t>D103</t>
-  </si>
-  <si>
-    <t>Length comps only</t>
-  </si>
-  <si>
-    <t>length and conditional age-at-length</t>
-  </si>
-  <si>
     <t>D0 but with CAL data</t>
   </si>
   <si>
-    <t>Same as D100 but without CAL</t>
-  </si>
-  <si>
-    <t>Same as D101 but w/o age data</t>
-  </si>
-  <si>
-    <t>Same as D100 but w/o age data</t>
-  </si>
-  <si>
     <t>Age and length comps, deterministic</t>
   </si>
   <si>
-    <t>Length and calcomps, deterministic</t>
+    <t>Binning cases</t>
+  </si>
+  <si>
+    <t>mac</t>
+  </si>
+  <si>
+    <t>yel</t>
+  </si>
+  <si>
+    <t>hak</t>
+  </si>
+  <si>
+    <t>1cm</t>
+  </si>
+  <si>
+    <t>B0</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>Length comps only, deterministic</t>
+  </si>
+  <si>
+    <t>length and calcomp, deterministic</t>
+  </si>
+  <si>
+    <t>Same as D100 but without age</t>
+  </si>
+  <si>
+    <t>Same as D101 but w/ calcomps</t>
+  </si>
+  <si>
+    <t>Fishing effort</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data </t>
+  </si>
+  <si>
+    <t>Estimation</t>
+  </si>
+  <si>
+    <t>Small bin width</t>
+  </si>
+  <si>
+    <t>Broad bin width</t>
+  </si>
+  <si>
+    <t>2cm</t>
+  </si>
+  <si>
+    <t>20cm</t>
+  </si>
+  <si>
+    <t>Set OM dat bins to 1cm; use with external cases</t>
+  </si>
+  <si>
+    <t>Internal cases</t>
+  </si>
+  <si>
+    <t>External cases</t>
+  </si>
+  <si>
+    <t>I0</t>
+  </si>
+  <si>
+    <t>I1</t>
+  </si>
+  <si>
+    <t>I2</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>No external binning; use with internal cases</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -189,6 +240,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -215,10 +274,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -524,255 +584,395 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G25"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="46" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B1" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="2:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F7" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7" t="s">
+        <v>45</v>
+      </c>
+      <c r="H7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:8" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12" t="s">
+        <v>43</v>
+      </c>
+      <c r="H12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G13" t="s">
+        <v>45</v>
+      </c>
+      <c r="H13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" t="s">
+        <v>55</v>
+      </c>
+      <c r="D14" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="1:7" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
         <v>0</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="2:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="E5" t="s">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>53</v>
+      </c>
+      <c r="E21" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="2:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
         <v>2</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C22" t="s">
         <v>22</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D22" t="s">
         <v>29</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E22" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="2:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
         <v>3</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C23" t="s">
         <v>23</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D23" t="s">
         <v>29</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E23" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="2:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
         <v>4</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C24" t="s">
         <v>24</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D24" t="s">
         <v>29</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E24" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="2:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
         <v>13</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C25" t="s">
         <v>24</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D25" t="s">
         <v>29</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E25" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="2:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
         <v>14</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C26" t="s">
         <v>30</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D26" t="s">
         <v>28</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E26" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="2:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
         <v>15</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C27" t="s">
         <v>30</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D27" t="s">
         <v>28</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E27" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="2:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
         <v>31</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C28" t="s">
         <v>34</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D28" t="s">
         <v>33</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E28" t="s">
         <v>26</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" t="s">
+        <v>35</v>
+      </c>
+      <c r="D29" t="s">
+        <v>33</v>
+      </c>
+      <c r="E29" t="s">
+        <v>27</v>
+      </c>
+      <c r="G29" s="1"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="13" spans="2:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13" t="s">
-        <v>33</v>
-      </c>
-      <c r="E13" t="s">
-        <v>27</v>
-      </c>
-      <c r="G13" s="1" t="s">
+      <c r="C30" t="s">
+        <v>40</v>
+      </c>
+      <c r="D30" t="s">
+        <v>39</v>
+      </c>
+      <c r="G30" s="1"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B14" t="s">
+      <c r="C31" t="s">
+        <v>48</v>
+      </c>
+      <c r="D31" t="s">
+        <v>50</v>
+      </c>
+      <c r="G31" s="1"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
         <v>38</v>
       </c>
-      <c r="C14" t="s">
-        <v>48</v>
-      </c>
-      <c r="D14" t="s">
-        <v>44</v>
-      </c>
-      <c r="G14" s="1"/>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B15" t="s">
-        <v>39</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="C32" t="s">
         <v>49</v>
       </c>
-      <c r="D15" t="s">
-        <v>45</v>
-      </c>
-      <c r="G15" s="1"/>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B16" t="s">
-        <v>40</v>
-      </c>
-      <c r="C16" t="s">
-        <v>42</v>
-      </c>
-      <c r="D16" t="s">
-        <v>46</v>
-      </c>
-      <c r="G16" s="1"/>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B17" t="s">
-        <v>41</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D17" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="2:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
+      <c r="D32" t="s">
+        <v>51</v>
+      </c>
+      <c r="G32" s="1"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C33" s="2"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
         <v>5</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C35" t="s">
         <v>7</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F35" t="s">
         <v>20</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G35" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="2:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
         <v>6</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C36" t="s">
         <v>17</v>
       </c>
-      <c r="F21">
+      <c r="F36">
         <f>47.4245*1.25</f>
         <v>59.280625000000001</v>
       </c>
     </row>
-    <row r="23" spans="2:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
         <v>9</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C38" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="2:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
         <v>11</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C39" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B25" t="s">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
         <v>18</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C40" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
switched from cod to cos model, was causing the weirdness
</commit_message>
<xml_diff>
--- a/case list.xlsx
+++ b/case list.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="684" yWindow="360" windowWidth="15984" windowHeight="6108"/>
+    <workbookView xWindow="680" yWindow="360" windowWidth="15980" windowHeight="6110"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="69">
   <si>
     <t>F0</t>
   </si>
@@ -215,6 +215,12 @@
   </si>
   <si>
     <t>No external binning; use with internal cases</t>
+  </si>
+  <si>
+    <t>change_em_binning</t>
+  </si>
+  <si>
+    <t>change_data</t>
   </si>
 </sst>
 </file>
@@ -587,28 +593,32 @@
   <dimension ref="A1:H40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C14" sqref="C14:D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="3" width="46" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B1" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>60</v>
       </c>
@@ -674,7 +684,11 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:8" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>67</v>
+      </c>
+    </row>
     <row r="12" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>61</v>
@@ -742,12 +756,12 @@
     </row>
     <row r="16" spans="1:8" ht="15" x14ac:dyDescent="0.25"/>
     <row r="17" spans="1:7" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>0</v>
       </c>
@@ -755,12 +769,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>53</v>
       </c>
@@ -768,7 +782,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>2</v>
       </c>
@@ -782,7 +796,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>3</v>
       </c>
@@ -796,7 +810,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>4</v>
       </c>
@@ -810,7 +824,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>13</v>
       </c>
@@ -824,7 +838,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>14</v>
       </c>
@@ -838,7 +852,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>15</v>
       </c>
@@ -852,7 +866,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
         <v>31</v>
       </c>
@@ -867,7 +881,7 @@
       </c>
       <c r="G28" s="1"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
         <v>32</v>
       </c>
@@ -882,7 +896,7 @@
       </c>
       <c r="G29" s="1"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
         <v>36</v>
       </c>
@@ -894,7 +908,7 @@
       </c>
       <c r="G30" s="1"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
         <v>37</v>
       </c>
@@ -906,7 +920,7 @@
       </c>
       <c r="G31" s="1"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
         <v>38</v>
       </c>
@@ -918,15 +932,15 @@
       </c>
       <c r="G32" s="1"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C33" s="2"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B35" t="s">
         <v>5</v>
       </c>
@@ -940,7 +954,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B36" t="s">
         <v>6</v>
       </c>
@@ -952,7 +966,7 @@
         <v>59.280625000000001</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B38" t="s">
         <v>9</v>
       </c>
@@ -960,7 +974,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B39" t="s">
         <v>11</v>
       </c>
@@ -968,7 +982,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B40" t="s">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
updated to remove internal binning and use external only
</commit_message>
<xml_diff>
--- a/case list.xlsx
+++ b/case list.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="58">
   <si>
     <t>F0</t>
   </si>
@@ -77,9 +77,6 @@
   </si>
   <si>
     <t>B2</t>
-  </si>
-  <si>
-    <t>No external binning; use with internal cases</t>
   </si>
   <si>
     <t>Length</t>
@@ -186,9 +183,6 @@
     <t>I3</t>
   </si>
   <si>
-    <t>1cm internal bins for use with external cases;</t>
-  </si>
-  <si>
     <t>External case, using the change_em_binning function</t>
   </si>
   <si>
@@ -202,6 +196,21 @@
   </si>
   <si>
     <t>E991</t>
+  </si>
+  <si>
+    <t>Pop bins match data bins for B1</t>
+  </si>
+  <si>
+    <t>Pop bins match data bins for B2</t>
+  </si>
+  <si>
+    <t>Pop bins match data bins for B3</t>
+  </si>
+  <si>
+    <t>Pop bins 1cm</t>
+  </si>
+  <si>
+    <t>1cm binning</t>
   </si>
 </sst>
 </file>
@@ -376,7 +385,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -439,6 +448,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -743,8 +753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -780,98 +790,21 @@
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>
       <c r="B5" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="E5" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="G5" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="H5" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="I5" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="J5" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="K5" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="L5" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="M5" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="N5" s="17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.35">
+        <v>45</v>
+      </c>
+      <c r="C5" s="29"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A6" s="2"/>
       <c r="B6" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="E6" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="F6" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="G6" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="H6" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="I6" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="J6" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="K6" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="L6" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="M6" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="N6" s="19" t="s">
-        <v>47</v>
+      <c r="C6" s="32" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
@@ -879,41 +812,8 @@
       <c r="B7" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="20">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="E7" s="27">
-        <v>2</v>
-      </c>
-      <c r="F7" s="20">
-        <v>1</v>
-      </c>
-      <c r="G7" s="20">
-        <v>1</v>
-      </c>
-      <c r="H7" s="20">
-        <v>1</v>
-      </c>
-      <c r="I7" s="21">
-        <v>1</v>
-      </c>
-      <c r="J7" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="K7" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="L7" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="M7" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="N7" s="21" t="s">
-        <v>10</v>
+      <c r="C7" s="30" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
@@ -921,83 +821,17 @@
       <c r="B8" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="D8" s="20">
-        <v>2.9000000000000001E-2</v>
-      </c>
-      <c r="E8" s="27">
-        <v>4</v>
-      </c>
-      <c r="F8" s="20">
-        <v>2</v>
-      </c>
-      <c r="G8" s="20">
-        <v>2</v>
-      </c>
-      <c r="H8" s="20">
-        <v>2</v>
-      </c>
-      <c r="I8" s="21">
-        <v>2</v>
-      </c>
-      <c r="J8" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="K8" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="L8" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="M8" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="N8" s="21" t="s">
-        <v>16</v>
+      <c r="C8" s="30" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" s="2"/>
       <c r="B9" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="22">
-        <v>9.1999999999999998E-2</v>
-      </c>
-      <c r="E9" s="28">
-        <v>13</v>
-      </c>
-      <c r="F9" s="22">
-        <v>5</v>
-      </c>
-      <c r="G9" s="22">
-        <v>5</v>
-      </c>
-      <c r="H9" s="22">
-        <v>6</v>
-      </c>
-      <c r="I9" s="23">
-        <v>6</v>
-      </c>
-      <c r="J9" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="K9" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="L9" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="M9" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="N9" s="23" t="s">
-        <v>44</v>
+        <v>47</v>
+      </c>
+      <c r="C9" s="31" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
@@ -1005,7 +839,7 @@
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -1019,11 +853,11 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B11" s="24" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E11" s="25" t="s">
         <v>5</v>
@@ -1062,40 +896,40 @@
         <v>11</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="E12" s="26" t="s">
-        <v>47</v>
+        <v>46</v>
+      </c>
+      <c r="E12" s="26">
+        <v>1</v>
       </c>
       <c r="F12" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G12" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H12" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I12" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J12" s="26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K12" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L12" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M12" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N12" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
@@ -1146,7 +980,7 @@
         <v>20</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D14" s="20">
         <v>2.9000000000000001E-2</v>
@@ -1173,7 +1007,7 @@
         <v>16</v>
       </c>
       <c r="L14" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M14" s="20" t="s">
         <v>16</v>
@@ -1184,7 +1018,7 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B15" s="14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C15" s="15" t="s">
         <v>15</v>
@@ -1208,19 +1042,19 @@
         <v>6</v>
       </c>
       <c r="J15" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="K15" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="L15" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="K15" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="L15" s="22" t="s">
-        <v>45</v>
-      </c>
       <c r="M15" s="22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N15" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -1238,7 +1072,7 @@
     </row>
     <row r="17" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A17" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
@@ -1249,7 +1083,7 @@
         <v>2</v>
       </c>
       <c r="D18" s="29" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
@@ -1257,19 +1091,19 @@
         <v>1</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D19" s="30"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B20" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="15" t="s">
-        <v>38</v>
-      </c>
       <c r="D20" s="31" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
@@ -1282,10 +1116,10 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F23" t="s">
         <v>4</v>
@@ -1296,38 +1130,38 @@
     </row>
     <row r="25" spans="1:8" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A25" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D26" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E26" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="F26" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F26" s="4" t="s">
+      <c r="G26" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D27" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H27" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="H27" s="3" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
@@ -1335,10 +1169,10 @@
         <v>1</v>
       </c>
       <c r="C28" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D28" s="5" t="s">
         <v>28</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>29</v>
       </c>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
@@ -1354,13 +1188,13 @@
         <v>2</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F29" s="5"/>
       <c r="G29" s="5">
@@ -1375,14 +1209,14 @@
         <v>3</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E30" s="5"/>
       <c r="F30" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G30" s="5">
         <v>2</v>
@@ -1396,10 +1230,10 @@
         <v>4</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
@@ -1415,13 +1249,13 @@
         <v>5</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F32" s="5"/>
       <c r="G32" s="5">
@@ -1436,14 +1270,14 @@
         <v>6</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E33" s="5"/>
       <c r="F33" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G33" s="5">
         <v>2</v>

</xml_diff>

<commit_message>
updated case files for new proposed bins
</commit_message>
<xml_diff>
--- a/case list.xlsx
+++ b/case list.xlsx
@@ -286,7 +286,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -598,19 +598,16 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
@@ -632,19 +629,19 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
@@ -659,6 +656,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -677,6 +677,1024 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Linf:Bin widths</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$M$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>cod</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$M$11:$M$15</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>7.575757575757576E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5151515151515152E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0303030303030304E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.0909090909090912E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.18181818181818182</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$N$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>fla</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$N$11:$N$15</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2.1086147455429156E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.2172294910858311E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.10543073727714578</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.21086147455429155</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4217229491085831</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$O$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>yel</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$O$11:$O$15</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1.6129032258064516E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.2258064516129031E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.4516129032258063E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.19354838709677419</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.38709677419354838</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="31297008"/>
+        <c:axId val="31296616"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="31297008"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="31296616"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="31296616"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="31297008"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>111125</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>41275</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>415925</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>168275</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -968,8 +1986,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1002,24 +2020,24 @@
       <c r="N3" s="2"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="C4" s="33" t="s">
+      <c r="C4" s="32" t="s">
         <v>75</v>
       </c>
-      <c r="D4" s="35" t="s">
+      <c r="D4" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="E4" s="33" t="s">
+      <c r="E4" s="32" t="s">
         <v>77</v>
       </c>
-      <c r="F4" s="35" t="s">
+      <c r="F4" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="G4" s="35" t="s">
+      <c r="G4" s="34" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B5" s="49" t="s">
+      <c r="B5" s="48" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="19">
@@ -1039,7 +2057,7 @@
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B6" s="50" t="s">
+      <c r="B6" s="49" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="20">
@@ -1059,7 +2077,7 @@
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B7" s="51" t="s">
+      <c r="B7" s="50" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="21">
@@ -1087,7 +2105,7 @@
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B9" s="52" t="s">
+      <c r="B9" s="51" t="s">
         <v>44</v>
       </c>
       <c r="C9" s="2"/>
@@ -1109,97 +2127,97 @@
       <c r="M9" s="2"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B10" s="40" t="s">
+      <c r="B10" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="41"/>
-      <c r="D10" s="33" t="s">
+      <c r="C10" s="40"/>
+      <c r="D10" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="34" t="s">
+      <c r="E10" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="F10" s="34" t="s">
+      <c r="F10" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="G10" s="33" t="s">
+      <c r="G10" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="H10" s="34" t="s">
+      <c r="H10" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="I10" s="35" t="s">
+      <c r="I10" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="J10" s="33" t="s">
+      <c r="J10" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="K10" s="34" t="s">
+      <c r="K10" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="L10" s="35" t="s">
+      <c r="L10" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="M10" s="33" t="s">
+      <c r="M10" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="N10" s="34" t="s">
+      <c r="N10" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="O10" s="35" t="s">
+      <c r="O10" s="34" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" s="2"/>
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="37" t="s">
+      <c r="C11" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="D11" s="39">
+      <c r="D11" s="38">
         <v>1</v>
       </c>
-      <c r="E11" s="38">
+      <c r="E11" s="37">
         <v>1</v>
       </c>
-      <c r="F11" s="38">
+      <c r="F11" s="37">
         <v>1</v>
       </c>
-      <c r="G11" s="39">
+      <c r="G11" s="38">
         <f>($D$5-$C$5)/D11</f>
         <v>192</v>
       </c>
-      <c r="H11" s="38">
+      <c r="H11" s="37">
         <f>($D$6-$C$6)/E11</f>
         <v>100</v>
       </c>
-      <c r="I11" s="38">
+      <c r="I11" s="37">
         <f>($D$7-$C$7)/F11</f>
         <v>96</v>
       </c>
-      <c r="J11" s="39">
+      <c r="J11" s="38">
         <f>($F$5-$E$5)/D11</f>
         <v>144</v>
       </c>
-      <c r="K11" s="38">
+      <c r="K11" s="37">
         <f>($F$6-$E$6)/E11</f>
         <v>60</v>
       </c>
-      <c r="L11" s="38">
+      <c r="L11" s="37">
         <f>($F$7-$E$7)/F11</f>
         <v>72</v>
       </c>
-      <c r="M11" s="42">
+      <c r="M11" s="41">
         <f>D11/$G$5</f>
         <v>7.575757575757576E-3</v>
       </c>
-      <c r="N11" s="43">
+      <c r="N11" s="42">
         <f>E11/$G$6</f>
         <v>2.1086147455429156E-2</v>
       </c>
-      <c r="O11" s="44">
+      <c r="O11" s="43">
         <f>F11/$G$7</f>
         <v>1.6129032258064516E-2</v>
       </c>
@@ -1245,15 +2263,15 @@
         <f>($F$7-$E$7)/F12</f>
         <v>36</v>
       </c>
-      <c r="M12" s="45">
+      <c r="M12" s="44">
         <f>D12/$G$5</f>
         <v>1.5151515151515152E-2</v>
       </c>
-      <c r="N12" s="29">
+      <c r="N12" s="28">
         <f>E12/$G$6</f>
         <v>4.2172294910858311E-2</v>
       </c>
-      <c r="O12" s="30">
+      <c r="O12" s="29">
         <f>F12/$G$7</f>
         <v>3.2258064516129031E-2</v>
       </c>
@@ -1273,7 +2291,7 @@
         <v>5</v>
       </c>
       <c r="F13" s="15">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G13" s="20">
         <f>($D$5-$C$5)/D13</f>
@@ -1285,7 +2303,7 @@
       </c>
       <c r="I13" s="15">
         <f>($D$7-$C$7)/F13</f>
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="J13" s="20">
         <f>($F$5-$E$5)/D13</f>
@@ -1297,19 +2315,19 @@
       </c>
       <c r="L13" s="15">
         <f>($F$7-$E$7)/F13</f>
-        <v>12</v>
-      </c>
-      <c r="M13" s="45">
+        <v>18</v>
+      </c>
+      <c r="M13" s="44">
         <f>D13/$G$5</f>
         <v>3.0303030303030304E-2</v>
       </c>
-      <c r="N13" s="29">
+      <c r="N13" s="28">
         <f>E13/$G$6</f>
         <v>0.10543073727714578</v>
       </c>
-      <c r="O13" s="30">
+      <c r="O13" s="29">
         <f>F13/$G$7</f>
-        <v>9.6774193548387094E-2</v>
+        <v>6.4516129032258063E-2</v>
       </c>
     </row>
     <row r="14" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -1352,15 +2370,15 @@
         <f>($F$7-$E$7)/F14</f>
         <v>6</v>
       </c>
-      <c r="M14" s="45">
+      <c r="M14" s="44">
         <f>D14/$G$5</f>
         <v>9.0909090909090912E-2</v>
       </c>
-      <c r="N14" s="29">
+      <c r="N14" s="28">
         <f>E14/$G$6</f>
         <v>0.21086147455429155</v>
       </c>
-      <c r="O14" s="30">
+      <c r="O14" s="29">
         <f>F14/$G$7</f>
         <v>0.19354838709677419</v>
       </c>
@@ -1405,15 +2423,15 @@
         <f>($F$7-$E$7)/F15</f>
         <v>3</v>
       </c>
-      <c r="M15" s="46">
+      <c r="M15" s="45">
         <f>D15/$G$5</f>
         <v>0.18181818181818182</v>
       </c>
-      <c r="N15" s="31">
+      <c r="N15" s="30">
         <f>E15/$G$6</f>
         <v>0.4217229491085831</v>
       </c>
-      <c r="O15" s="32">
+      <c r="O15" s="31">
         <f>F15/$G$7</f>
         <v>0.38709677419354838</v>
       </c>
@@ -1481,10 +2499,10 @@
       <c r="N19" s="15"/>
     </row>
     <row r="20" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="47" t="s">
+      <c r="B20" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="48" t="s">
+      <c r="C20" s="47" t="s">
         <v>72</v>
       </c>
       <c r="D20" s="15"/>
@@ -1807,7 +2825,7 @@
       <c r="C48" t="s">
         <v>51</v>
       </c>
-      <c r="D48" s="28" t="s">
+      <c r="D48" s="52" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1818,7 +2836,7 @@
       <c r="C49" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D49" s="28"/>
+      <c r="D49" s="52"/>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B50">
@@ -1827,7 +2845,7 @@
       <c r="C50" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D50" s="28"/>
+      <c r="D50" s="52"/>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B51">
@@ -1836,7 +2854,7 @@
       <c r="C51" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D51" s="28"/>
+      <c r="D51" s="52"/>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B52">
@@ -1845,7 +2863,7 @@
       <c r="C52" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D52" s="28"/>
+      <c r="D52" s="52"/>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B53">
@@ -1854,7 +2872,7 @@
       <c r="C53" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D53" s="28"/>
+      <c r="D53" s="52"/>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B54">
@@ -1863,7 +2881,7 @@
       <c r="C54" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D54" s="28" t="s">
+      <c r="D54" s="52" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1874,7 +2892,7 @@
       <c r="C55" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D55" s="28"/>
+      <c r="D55" s="52"/>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B56" s="2">
@@ -1883,7 +2901,7 @@
       <c r="C56" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D56" s="28"/>
+      <c r="D56" s="52"/>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B57" s="2">
@@ -1892,7 +2910,7 @@
       <c r="C57" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D57" s="28"/>
+      <c r="D57" s="52"/>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B58" s="2">
@@ -1901,7 +2919,7 @@
       <c r="C58" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D58" s="28"/>
+      <c r="D58" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1910,5 +2928,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update to run different set of bin scenarios
</commit_message>
<xml_diff>
--- a/case list.xlsx
+++ b/case list.xlsx
@@ -1,25 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Cole\binning\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="680" yWindow="360" windowWidth="15980" windowHeight="6110"/>
+    <workbookView xWindow="684" yWindow="360" windowWidth="15984" windowHeight="6108"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" iterateDelta="1E-4"/>
+  <calcPr calcId="145621" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="80">
   <si>
     <t>F0</t>
   </si>
@@ -279,6 +274,9 @@
   </si>
   <si>
     <t>max data bin</t>
+  </si>
+  <si>
+    <t>Base case</t>
   </si>
 </sst>
 </file>
@@ -353,7 +351,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -363,6 +361,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -545,7 +549,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -659,6 +663,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -728,26 +736,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -919,12 +907,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="31297008"/>
-        <c:axId val="31296616"/>
+        <c:axId val="136914048"/>
+        <c:axId val="136915584"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="31297008"/>
+        <c:axId val="136914048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -966,7 +955,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="31296616"/>
+        <c:crossAx val="136915584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -974,7 +963,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="31296616"/>
+        <c:axId val="136915584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1025,7 +1014,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="31297008"/>
+        <c:crossAx val="136914048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1740,7 +1729,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1775,7 +1764,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1986,31 +1975,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.1796875" customWidth="1"/>
-    <col min="2" max="2" width="17.1796875" customWidth="1"/>
-    <col min="3" max="3" width="33.453125" customWidth="1"/>
-    <col min="4" max="4" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.21875" customWidth="1"/>
+    <col min="2" max="2" width="17.21875" customWidth="1"/>
+    <col min="3" max="3" width="33.44140625" customWidth="1"/>
+    <col min="4" max="4" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:15" ht="18.45" x14ac:dyDescent="0.45">
       <c r="B1" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" ht="15.45" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" ht="14.55" x14ac:dyDescent="0.35">
       <c r="C3" t="s">
         <v>66</v>
       </c>
@@ -2019,7 +2008,7 @@
       </c>
       <c r="N3" s="2"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" ht="14.55" x14ac:dyDescent="0.35">
       <c r="C4" s="32" t="s">
         <v>75</v>
       </c>
@@ -2036,7 +2025,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" ht="14.55" x14ac:dyDescent="0.35">
       <c r="B5" s="48" t="s">
         <v>5</v>
       </c>
@@ -2056,7 +2045,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" ht="14.55" x14ac:dyDescent="0.35">
       <c r="B6" s="49" t="s">
         <v>4</v>
       </c>
@@ -2076,7 +2065,7 @@
         <v>47.424500000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" ht="14.55" x14ac:dyDescent="0.35">
       <c r="B7" s="50" t="s">
         <v>7</v>
       </c>
@@ -2096,7 +2085,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" ht="15.45" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
         <v>6</v>
       </c>
@@ -2104,7 +2093,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" ht="14.55" x14ac:dyDescent="0.35">
       <c r="B9" s="51" t="s">
         <v>44</v>
       </c>
@@ -2126,7 +2115,7 @@
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" ht="14.55" x14ac:dyDescent="0.35">
       <c r="B10" s="39" t="s">
         <v>34</v>
       </c>
@@ -2168,7 +2157,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" ht="14.55" x14ac:dyDescent="0.35">
       <c r="A11" s="2"/>
       <c r="B11" s="35" t="s">
         <v>8</v>
@@ -2222,7 +2211,7 @@
         <v>1.6129032258064516E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" ht="14.55" x14ac:dyDescent="0.35">
       <c r="A12" s="2"/>
       <c r="B12" s="10" t="s">
         <v>9</v>
@@ -2276,7 +2265,7 @@
         <v>3.2258064516129031E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:15" ht="14.55" x14ac:dyDescent="0.35">
       <c r="A13" s="2"/>
       <c r="B13" s="10" t="s">
         <v>14</v>
@@ -2330,7 +2319,7 @@
         <v>6.4516129032258063E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:15" s="2" customFormat="1" ht="14.55" x14ac:dyDescent="0.35">
       <c r="B14" s="10" t="s">
         <v>36</v>
       </c>
@@ -2383,7 +2372,7 @@
         <v>0.19354838709677419</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:15" ht="14.55" x14ac:dyDescent="0.35">
       <c r="B15" s="12" t="s">
         <v>64</v>
       </c>
@@ -2436,7 +2425,7 @@
         <v>0.38709677419354838</v>
       </c>
     </row>
-    <row r="16" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" s="2" customFormat="1" ht="14.55" x14ac:dyDescent="0.35">
       <c r="D16" s="15"/>
       <c r="E16" s="15"/>
       <c r="F16" s="15"/>
@@ -2448,7 +2437,7 @@
       <c r="L16" s="15"/>
       <c r="M16" s="15"/>
     </row>
-    <row r="17" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" s="2" customFormat="1" ht="14.55" x14ac:dyDescent="0.35">
       <c r="A17"/>
       <c r="B17" s="26" t="s">
         <v>43</v>
@@ -2465,7 +2454,7 @@
       <c r="M17" s="15"/>
       <c r="N17" s="15"/>
     </row>
-    <row r="18" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14" s="2" customFormat="1" ht="14.55" x14ac:dyDescent="0.35">
       <c r="B18" s="27" t="s">
         <v>46</v>
       </c>
@@ -2481,7 +2470,7 @@
       <c r="M18" s="15"/>
       <c r="N18" s="15"/>
     </row>
-    <row r="19" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:14" s="2" customFormat="1" ht="14.55" x14ac:dyDescent="0.35">
       <c r="B19" s="8" t="s">
         <v>33</v>
       </c>
@@ -2498,7 +2487,7 @@
       <c r="M19" s="15"/>
       <c r="N19" s="15"/>
     </row>
-    <row r="20" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14" s="2" customFormat="1" ht="14.55" x14ac:dyDescent="0.35">
       <c r="B20" s="46" t="s">
         <v>13</v>
       </c>
@@ -2517,7 +2506,7 @@
       <c r="M20" s="15"/>
       <c r="N20" s="15"/>
     </row>
-    <row r="21" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:14" s="2" customFormat="1" ht="14.55" x14ac:dyDescent="0.35">
       <c r="D21" s="15"/>
       <c r="E21" s="15"/>
       <c r="F21" s="15"/>
@@ -2530,7 +2519,7 @@
       <c r="M21" s="15"/>
       <c r="N21" s="15"/>
     </row>
-    <row r="22" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:14" ht="15.45" x14ac:dyDescent="0.35">
       <c r="A22" s="6" t="s">
         <v>47</v>
       </c>
@@ -2538,12 +2527,12 @@
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:14" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:14" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.35">
       <c r="A23" s="6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:14" ht="14.55" x14ac:dyDescent="0.35">
       <c r="B24" s="8" t="s">
         <v>0</v>
       </c>
@@ -2554,7 +2543,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:14" ht="14.55" x14ac:dyDescent="0.35">
       <c r="B25" s="10" t="s">
         <v>1</v>
       </c>
@@ -2563,7 +2552,7 @@
       </c>
       <c r="D25" s="23"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:14" ht="14.55" x14ac:dyDescent="0.35">
       <c r="B26" s="12" t="s">
         <v>29</v>
       </c>
@@ -2574,10 +2563,10 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:14" ht="14.55" x14ac:dyDescent="0.35">
       <c r="C27" s="1"/>
     </row>
-    <row r="28" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:14" ht="15.45" x14ac:dyDescent="0.35">
       <c r="A28" s="6" t="s">
         <v>10</v>
       </c>
@@ -2585,7 +2574,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>38</v>
       </c>
@@ -2599,7 +2588,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:14" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:14" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
         <v>32</v>
       </c>
@@ -2607,7 +2596,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D32" s="4" t="s">
         <v>15</v>
       </c>
@@ -2621,7 +2610,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D33" s="3" t="s">
         <v>19</v>
       </c>
@@ -2638,26 +2627,26 @@
         <v>20</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B34" s="2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B34" s="53">
         <v>1</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C34" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="D34" s="54" t="s">
         <v>22</v>
       </c>
-      <c r="E34" s="5"/>
-      <c r="F34" s="5"/>
-      <c r="G34" s="5">
+      <c r="E34" s="54"/>
+      <c r="F34" s="54"/>
+      <c r="G34" s="54">
         <v>2</v>
       </c>
-      <c r="H34" s="2">
+      <c r="H34" s="53">
         <v>500</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B35" s="2">
         <v>2</v>
       </c>
@@ -2678,7 +2667,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B36" s="2">
         <v>3</v>
       </c>
@@ -2699,26 +2688,26 @@
         <v>500</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B37" s="2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B37" s="53">
         <v>4</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C37" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="D37" s="5" t="s">
+      <c r="D37" s="54" t="s">
         <v>22</v>
       </c>
-      <c r="E37" s="5"/>
-      <c r="F37" s="5"/>
-      <c r="G37" s="5">
+      <c r="E37" s="54"/>
+      <c r="F37" s="54"/>
+      <c r="G37" s="54">
         <v>2</v>
       </c>
-      <c r="H37" s="2">
+      <c r="H37" s="53">
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B38" s="2">
         <v>5</v>
       </c>
@@ -2739,7 +2728,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B39" s="2">
         <v>6</v>
       </c>
@@ -2760,49 +2749,49 @@
         <v>20</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B40">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B40" s="53">
         <v>7</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C40" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="D40" s="5" t="s">
+      <c r="D40" s="54" t="s">
         <v>22</v>
       </c>
-      <c r="E40" s="5" t="s">
+      <c r="E40" s="54" t="s">
         <v>22</v>
       </c>
-      <c r="F40" s="5"/>
-      <c r="G40" s="5">
+      <c r="F40" s="54"/>
+      <c r="G40" s="54">
         <v>2</v>
       </c>
-      <c r="H40" s="2" t="s">
+      <c r="H40" s="53" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B41">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B41" s="53">
         <v>8</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C41" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="D41" s="5" t="s">
+      <c r="D41" s="54" t="s">
         <v>22</v>
       </c>
-      <c r="E41" s="5"/>
-      <c r="F41" s="5" t="s">
+      <c r="E41" s="54"/>
+      <c r="F41" s="54" t="s">
         <v>22</v>
       </c>
-      <c r="G41" s="5">
+      <c r="G41" s="54">
         <v>2</v>
       </c>
-      <c r="H41" s="2" t="s">
+      <c r="H41" s="53" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="25" t="s">
         <v>41</v>
       </c>
@@ -2810,15 +2799,18 @@
         <v>46</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B47">
         <v>0</v>
       </c>
       <c r="C47" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D47" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B48">
         <v>11</v>
       </c>
@@ -2829,7 +2821,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B49">
         <v>12</v>
       </c>
@@ -2838,7 +2830,7 @@
       </c>
       <c r="D49" s="52"/>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B50">
         <v>13</v>
       </c>
@@ -2847,7 +2839,7 @@
       </c>
       <c r="D50" s="52"/>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B51">
         <v>14</v>
       </c>
@@ -2856,7 +2848,7 @@
       </c>
       <c r="D51" s="52"/>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B52">
         <v>15</v>
       </c>
@@ -2865,7 +2857,7 @@
       </c>
       <c r="D52" s="52"/>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B53">
         <v>16</v>
       </c>
@@ -2874,7 +2866,7 @@
       </c>
       <c r="D53" s="52"/>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B54">
         <v>21</v>
       </c>
@@ -2885,7 +2877,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B55">
         <v>22</v>
       </c>
@@ -2894,7 +2886,7 @@
       </c>
       <c r="D55" s="52"/>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B56" s="2">
         <v>23</v>
       </c>
@@ -2903,7 +2895,7 @@
       </c>
       <c r="D56" s="52"/>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B57" s="2">
         <v>24</v>
       </c>
@@ -2912,7 +2904,7 @@
       </c>
       <c r="D57" s="52"/>
     </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B58" s="2">
         <v>25</v>
       </c>

</xml_diff>

<commit_message>
updated cases to have data bin ranges match pop bins ranges
</commit_message>
<xml_diff>
--- a/case list.xlsx
+++ b/case list.xlsx
@@ -662,11 +662,11 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -909,11 +909,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="136914048"/>
-        <c:axId val="136915584"/>
+        <c:axId val="139928704"/>
+        <c:axId val="139930240"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="136914048"/>
+        <c:axId val="139928704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -955,7 +955,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="136915584"/>
+        <c:crossAx val="139930240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -963,7 +963,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="136915584"/>
+        <c:axId val="139930240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1014,7 +1014,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="136914048"/>
+        <c:crossAx val="139928704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1975,8 +1975,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2036,10 +2036,12 @@
         <v>200</v>
       </c>
       <c r="E5" s="19">
-        <v>20</v>
+        <f>C5</f>
+        <v>8</v>
       </c>
       <c r="F5" s="14">
-        <v>164</v>
+        <f t="shared" ref="F5:F7" si="0">D5</f>
+        <v>200</v>
       </c>
       <c r="G5" s="14">
         <v>132</v>
@@ -2056,10 +2058,12 @@
         <v>102</v>
       </c>
       <c r="E6" s="20">
-        <v>10</v>
+        <f t="shared" ref="E6:E7" si="1">C6</f>
+        <v>2</v>
       </c>
       <c r="F6" s="16">
-        <v>70</v>
+        <f t="shared" si="0"/>
+        <v>102</v>
       </c>
       <c r="G6" s="23">
         <v>47.424500000000002</v>
@@ -2076,14 +2080,37 @@
         <v>106</v>
       </c>
       <c r="E7" s="21">
-        <v>18</v>
+        <f t="shared" si="1"/>
+        <v>10</v>
       </c>
       <c r="F7" s="18">
-        <v>90</v>
+        <f t="shared" si="0"/>
+        <v>106</v>
       </c>
       <c r="G7" s="18">
         <v>62</v>
       </c>
+      <c r="I7">
+        <f>C7</f>
+        <v>10</v>
+      </c>
+      <c r="J7">
+        <f>I7+24</f>
+        <v>34</v>
+      </c>
+      <c r="K7" s="2">
+        <f t="shared" ref="K7:N7" si="2">J7+24</f>
+        <v>58</v>
+      </c>
+      <c r="L7" s="2">
+        <f t="shared" si="2"/>
+        <v>82</v>
+      </c>
+      <c r="M7" s="2">
+        <f t="shared" si="2"/>
+        <v>106</v>
+      </c>
+      <c r="N7" s="2"/>
     </row>
     <row r="8" spans="1:15" ht="15.45" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
@@ -2188,15 +2215,15 @@
       </c>
       <c r="J11" s="38">
         <f>($F$5-$E$5)/D11</f>
-        <v>144</v>
+        <v>192</v>
       </c>
       <c r="K11" s="37">
         <f>($F$6-$E$6)/E11</f>
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="L11" s="37">
         <f>($F$7-$E$7)/F11</f>
-        <v>72</v>
+        <v>96</v>
       </c>
       <c r="M11" s="41">
         <f>D11/$G$5</f>
@@ -2242,15 +2269,15 @@
       </c>
       <c r="J12" s="20">
         <f>($F$5-$E$5)/D12</f>
-        <v>72</v>
+        <v>96</v>
       </c>
       <c r="K12" s="15">
         <f>($F$6-$E$6)/E12</f>
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="L12" s="15">
         <f>($F$7-$E$7)/F12</f>
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="M12" s="44">
         <f>D12/$G$5</f>
@@ -2296,15 +2323,15 @@
       </c>
       <c r="J13" s="20">
         <f>($F$5-$E$5)/D13</f>
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="K13" s="15">
         <f>($F$6-$E$6)/E13</f>
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="L13" s="15">
         <f>($F$7-$E$7)/F13</f>
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="M13" s="44">
         <f>D13/$G$5</f>
@@ -2349,15 +2376,15 @@
       </c>
       <c r="J14" s="20">
         <f>($F$5-$E$5)/D14</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="K14" s="15">
         <f>($F$6-$E$6)/E14</f>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="L14" s="15">
         <f>($F$7-$E$7)/F14</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="M14" s="44">
         <f>D14/$G$5</f>
@@ -2402,15 +2429,15 @@
       </c>
       <c r="J15" s="21">
         <f>($F$5-$E$5)/D15</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="K15" s="17">
         <f>($F$6-$E$6)/E15</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="L15" s="17">
         <f>($F$7-$E$7)/F15</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M15" s="45">
         <f>D15/$G$5</f>
@@ -2628,21 +2655,21 @@
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B34" s="53">
+      <c r="B34" s="52">
         <v>1</v>
       </c>
-      <c r="C34" s="53" t="s">
+      <c r="C34" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="D34" s="54" t="s">
+      <c r="D34" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="E34" s="54"/>
-      <c r="F34" s="54"/>
-      <c r="G34" s="54">
+      <c r="E34" s="53"/>
+      <c r="F34" s="53"/>
+      <c r="G34" s="53">
         <v>2</v>
       </c>
-      <c r="H34" s="53">
+      <c r="H34" s="52">
         <v>500</v>
       </c>
     </row>
@@ -2689,21 +2716,21 @@
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B37" s="53">
+      <c r="B37" s="52">
         <v>4</v>
       </c>
-      <c r="C37" s="53" t="s">
+      <c r="C37" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="D37" s="54" t="s">
+      <c r="D37" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="E37" s="54"/>
-      <c r="F37" s="54"/>
-      <c r="G37" s="54">
+      <c r="E37" s="53"/>
+      <c r="F37" s="53"/>
+      <c r="G37" s="53">
         <v>2</v>
       </c>
-      <c r="H37" s="53">
+      <c r="H37" s="52">
         <v>20</v>
       </c>
     </row>
@@ -2750,44 +2777,44 @@
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B40" s="53">
+      <c r="B40" s="52">
         <v>7</v>
       </c>
-      <c r="C40" s="53" t="s">
+      <c r="C40" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="D40" s="54" t="s">
+      <c r="D40" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="E40" s="54" t="s">
+      <c r="E40" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="F40" s="54"/>
-      <c r="G40" s="54">
+      <c r="F40" s="53"/>
+      <c r="G40" s="53">
         <v>2</v>
       </c>
-      <c r="H40" s="53" t="s">
+      <c r="H40" s="52" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B41" s="53">
+      <c r="B41" s="52">
         <v>8</v>
       </c>
-      <c r="C41" s="53" t="s">
+      <c r="C41" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="D41" s="54" t="s">
+      <c r="D41" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="E41" s="54"/>
-      <c r="F41" s="54" t="s">
+      <c r="E41" s="53"/>
+      <c r="F41" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="G41" s="54">
+      <c r="G41" s="53">
         <v>2</v>
       </c>
-      <c r="H41" s="53" t="s">
+      <c r="H41" s="52" t="s">
         <v>40</v>
       </c>
     </row>
@@ -2817,7 +2844,7 @@
       <c r="C48" t="s">
         <v>51</v>
       </c>
-      <c r="D48" s="52" t="s">
+      <c r="D48" s="54" t="s">
         <v>62</v>
       </c>
     </row>
@@ -2828,7 +2855,7 @@
       <c r="C49" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D49" s="52"/>
+      <c r="D49" s="54"/>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B50">
@@ -2837,7 +2864,7 @@
       <c r="C50" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D50" s="52"/>
+      <c r="D50" s="54"/>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B51">
@@ -2846,7 +2873,7 @@
       <c r="C51" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D51" s="52"/>
+      <c r="D51" s="54"/>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B52">
@@ -2855,7 +2882,7 @@
       <c r="C52" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D52" s="52"/>
+      <c r="D52" s="54"/>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B53">
@@ -2864,7 +2891,7 @@
       <c r="C53" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D53" s="52"/>
+      <c r="D53" s="54"/>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B54">
@@ -2873,7 +2900,7 @@
       <c r="C54" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D54" s="52" t="s">
+      <c r="D54" s="54" t="s">
         <v>63</v>
       </c>
     </row>
@@ -2884,7 +2911,7 @@
       <c r="C55" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D55" s="52"/>
+      <c r="D55" s="54"/>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B56" s="2">
@@ -2893,7 +2920,7 @@
       <c r="C56" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D56" s="52"/>
+      <c r="D56" s="54"/>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B57" s="2">
@@ -2902,7 +2929,7 @@
       <c r="C57" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D57" s="52"/>
+      <c r="D57" s="54"/>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B58" s="2">
@@ -2911,7 +2938,7 @@
       <c r="C58" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D58" s="52"/>
+      <c r="D58" s="54"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>